<commit_message>
Gestion de la barre de vie en général, ajout d'un background (exemple)
Gestion des dégats (perte et regain de vie)
</commit_message>
<xml_diff>
--- a/journaux_activite/Cahier personnel d'activité Valentin.xlsx
+++ b/journaux_activite/Cahier personnel d'activité Valentin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentin\Documents\Weird Fishes\MP_SFL_2019_G3_Weird_Fishes\journaux_activite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D680BB-5AB4-444D-B05B-4E6946E81B0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490BC49B-A2DA-4195-9C12-605AB6E82FB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>Planification G3 Weird Fishes</t>
   </si>
@@ -120,13 +120,37 @@
   </si>
   <si>
     <t>4,5</t>
+  </si>
+  <si>
+    <t>Poursuivre le système de vie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Faire réagir dégats/baisse de la barre de vie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Créer l'évènement "mort" et afficher écran Game Over</t>
+  </si>
+  <si>
+    <t>Afficher le background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     Ajout du statut Current Health et Max Health dans le script "Health Bar"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     Ajout de la condition if(Current Health == 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     Création du scripth "Health Bar"</t>
+  </si>
+  <si>
+    <t>6,5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,8 +173,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +218,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -215,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -273,6 +316,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -845,63 +897,90 @@
       <c r="A19" s="19">
         <v>5</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="7">
+        <v>3</v>
+      </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="18"/>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="18">
+        <v>2</v>
+      </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="7"/>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="18"/>
+      <c r="B23" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="7"/>
+      <c r="B24" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="18"/>
+      <c r="B25" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
-      <c r="B26" s="10"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -1172,12 +1251,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1339,15 +1415,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{479B6FBB-881D-490F-81F1-A2B484DCF3A4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7AE4B74-71BC-453A-8415-ED91EE087DA5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1371,10 +1451,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7AE4B74-71BC-453A-8415-ED91EE087DA5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{479B6FBB-881D-490F-81F1-A2B484DCF3A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>